<commit_message>
Update EDSD - Digital Demography office hours.xlsx
</commit_message>
<xml_diff>
--- a/Office hours/EDSD - Digital Demography office hours.xlsx
+++ b/Office hours/EDSD - Digital Demography office hours.xlsx
@@ -45,13 +45,13 @@
     <t>14.45 - 15.00</t>
   </si>
   <si>
-    <t>Jesus</t>
-  </si>
-  <si>
     <t>Online office hours for EDSD - Digital Demography week</t>
   </si>
   <si>
     <t>Diego Alburez-Gutierrez</t>
+  </si>
+  <si>
+    <t>Daniel</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,12 +464,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -495,7 +495,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -507,7 +507,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>

</xml_diff>